<commit_message>
Fixed issue with the code not running from feature level but running from scenario level.
</commit_message>
<xml_diff>
--- a/SalemQA/Features/data.xlsx
+++ b/SalemQA/Features/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SalemQA\SalemQA\Features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C9AAD3-B7DA-4683-A2C9-4184242EBEE9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32FE6BDB-4031-4A4B-85F5-C439ABC44B6A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="2136" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>orgusername</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>rahul66666666666@gmail.com</t>
+  </si>
+  <si>
+    <t>org</t>
+  </si>
+  <si>
+    <t>NathCorp</t>
   </si>
 </sst>
 </file>
@@ -400,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -412,20 +418,26 @@
     <col min="2" max="2" width="24.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>